<commit_message>
HW05 Q4.3 & Bonus
</commit_message>
<xml_diff>
--- a/Homework/HW05/TimeVsN.xlsx
+++ b/Homework/HW05/TimeVsN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liwei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EAEE7C6B-DAAE-443E-A3F5-5680C3D7A337}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BBFFF171-8587-4BAD-B442-7972EB2629FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10755" xr2:uid="{1EE5F00B-86E2-4AC5-A61B-E991F5DB39ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>n</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,42 @@
   </si>
   <si>
     <t>Throughput</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6600U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Newriver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time (CPU)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Throughput (CPU)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time (CUDA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Throughput (CUDA)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -82,8 +118,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -188,7 +227,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -223,7 +262,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -250,7 +289,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -580,7 +619,1289 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Time vs n (CUDA)</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (CPU)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>217.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-17EA-462F-9BD0-7EFFE280C204}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (CUDA)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-17EA-462F-9BD0-7EFFE280C204}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1616140991"/>
+        <c:axId val="1615846719"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1616140991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>n</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1615846719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1615846719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1616140991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Throughput</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> vs n (CUDA)</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (CPU)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>212438</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>194280</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>161393</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>149518</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130789</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D94C-4117-9948-7150DDE757C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (CUDA)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$22:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3205040</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6184600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10837100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20682200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34046200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56893100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D94C-4117-9948-7150DDE757C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1612533647"/>
+        <c:axId val="1616205183"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1612533647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>n</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1616205183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1616205183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1612533647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1136,19 +2457,1051 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>111918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1169,6 +3522,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121442</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>159542</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A36EE8-D6DB-4AC7-B89F-4CEB9B966800}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>245267</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>283367</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A41A9A0-4ADA-4250-9460-8E38D60EAFBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1474,92 +3899,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37203F5A-16FD-48E3-BC29-58325662B964}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.06640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>2.6093799999999998</v>
-      </c>
-      <c r="C2">
-        <v>214250</v>
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>7.875</v>
+        <v>2.6093799999999998</v>
       </c>
       <c r="C3">
-        <v>188483</v>
+        <v>214250</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>15.75</v>
+        <v>7.875</v>
       </c>
       <c r="C4">
-        <v>165137</v>
+        <v>188483</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>27.171900000000001</v>
+        <v>15.75</v>
       </c>
       <c r="C5">
-        <v>171236</v>
+        <v>165137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>79.859399999999994</v>
+        <v>27.171900000000001</v>
       </c>
       <c r="C6">
-        <v>144951</v>
+        <v>171236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>79.859399999999994</v>
+      </c>
+      <c r="C7">
+        <v>144951</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
         <v>25</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>224.96899999999999</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>126447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>3.47</v>
+      </c>
+      <c r="C22">
+        <v>212438</v>
+      </c>
+      <c r="D22">
+        <v>0.23</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3205040</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>7.64</v>
+      </c>
+      <c r="C23">
+        <v>194280</v>
+      </c>
+      <c r="D23">
+        <v>0.24</v>
+      </c>
+      <c r="E23" s="1">
+        <v>6184600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>14.44</v>
+      </c>
+      <c r="C24">
+        <v>180118</v>
+      </c>
+      <c r="D24">
+        <v>0.24</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10837100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>34.6</v>
+      </c>
+      <c r="C25">
+        <v>161393</v>
+      </c>
+      <c r="D25">
+        <v>0.27</v>
+      </c>
+      <c r="E25" s="1">
+        <v>20682200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>77.42</v>
+      </c>
+      <c r="C26">
+        <v>149518</v>
+      </c>
+      <c r="D26">
+        <v>0.34</v>
+      </c>
+      <c r="E26" s="1">
+        <v>34046200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>217.5</v>
+      </c>
+      <c r="C27">
+        <v>130789</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>56893100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>